<commit_message>
Placement des portes de partout et début d'une animation pour ouvrir la porte
</commit_message>
<xml_diff>
--- a/Types de Murs Possibles.xlsx
+++ b/Types de Murs Possibles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\INFO5\Bibliotheque_de_developpement_multimedia\Labyrinthe3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3593012A-827C-404E-B76A-582F5804F7FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1830FBD-E9F8-4497-9C32-29A8EFC56B6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="3" xr2:uid="{3C8390C5-9047-4A19-85FD-4E1F16ACA795}"/>
   </bookViews>
@@ -398,9 +398,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,9 +458,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,6 +469,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,7 +793,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:G5"/>
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -802,15 +802,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E2" s="14"/>
@@ -821,14 +821,14 @@
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="16"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="14"/>
@@ -840,10 +840,10 @@
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="25"/>
+      <c r="C4" s="16"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -854,9 +854,9 @@
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="14"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="22"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -878,14 +878,14 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="20"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="16"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -897,8 +897,8 @@
       <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="E9" s="28"/>
+      <c r="C9" s="16"/>
+      <c r="E9" s="27"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
     </row>
@@ -908,20 +908,20 @@
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="14"/>
-      <c r="E10" s="29"/>
+      <c r="E10" s="28"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="33"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="36"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="16"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
@@ -930,8 +930,8 @@
       <c r="B14" s="4">
         <v>0</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="16"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
@@ -941,9 +941,9 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="14"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="33"/>
+      <c r="G15" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F52C247-5647-44DB-BC11-3B36A81F1A11}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,27 +972,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
@@ -1004,9 +1004,9 @@
       <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="25"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11"/>
@@ -1014,9 +1014,9 @@
         <v>0</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="22"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
@@ -1032,14 +1032,14 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
@@ -1058,9 +1058,9 @@
       <c r="C9" s="4">
         <v>0</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="25"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="24"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
@@ -1075,9 +1075,9 @@
         <v>0</v>
       </c>
       <c r="C10" s="12"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="22"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="21"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
@@ -1107,14 +1107,14 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
@@ -1126,9 +1126,9 @@
       <c r="C14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="25"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="11"/>
@@ -1136,9 +1136,9 @@
         <v>0</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="22"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1160,14 +1160,14 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -1197,7 +1197,7 @@
       <c r="C20" s="12"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="33"/>
+      <c r="G20" s="32"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1216,14 +1216,14 @@
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="35"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -1250,7 +1250,7 @@
       <c r="C25" s="12"/>
       <c r="E25" s="8"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="33"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
@@ -1259,14 +1259,14 @@
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
@@ -1290,7 +1290,7 @@
       <c r="C30" s="12"/>
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="33"/>
+      <c r="G30" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1321,23 +1321,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="C4" s="13"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="35"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -1359,9 +1359,9 @@
       <c r="C5" s="7">
         <v>0</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="40"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="11"/>
@@ -1370,8 +1370,8 @@
       </c>
       <c r="C6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
@@ -1379,11 +1379,11 @@
       <c r="C7" s="14"/>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -1402,9 +1402,9 @@
         <v>0</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="20"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -1424,9 +1424,9 @@
       <c r="C11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -1442,9 +1442,9 @@
         <v>0</v>
       </c>
       <c r="C12" s="12"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="22"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="21"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -1461,11 +1461,11 @@
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="18"/>
+      <c r="H13" s="17"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="18"/>
+      <c r="L13" s="17"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
@@ -1477,29 +1477,29 @@
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="18"/>
+      <c r="H14" s="17"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="18"/>
+      <c r="L14" s="17"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="18"/>
+      <c r="H15" s="17"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="18"/>
+      <c r="L15" s="17"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
@@ -1510,14 +1510,14 @@
         <v>0</v>
       </c>
       <c r="C16" s="13"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="17"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="18"/>
+      <c r="L16" s="17"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
@@ -1532,14 +1532,14 @@
       <c r="C17" s="7">
         <v>0</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="18"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="18"/>
+      <c r="L17" s="17"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
@@ -1550,14 +1550,14 @@
         <v>0</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="18"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="17"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="18"/>
+      <c r="L18" s="17"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
@@ -1569,11 +1569,11 @@
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="18"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
-      <c r="L19" s="18"/>
+      <c r="L19" s="17"/>
       <c r="M19" s="14"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
@@ -1585,29 +1585,29 @@
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="18"/>
+      <c r="H20" s="17"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
-      <c r="L20" s="18"/>
+      <c r="L20" s="17"/>
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="18"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
-      <c r="L21" s="18"/>
+      <c r="L21" s="17"/>
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
@@ -1618,14 +1618,14 @@
         <v>0</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="17"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
-      <c r="L22" s="18"/>
+      <c r="L22" s="17"/>
       <c r="M22" s="14"/>
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
@@ -1640,14 +1640,14 @@
       <c r="C23" s="7">
         <v>0</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="18"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
-      <c r="L23" s="18"/>
+      <c r="L23" s="17"/>
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
       <c r="O23" s="14"/>
@@ -1658,14 +1658,14 @@
         <v>0</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="18"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="17"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
-      <c r="L24" s="18"/>
+      <c r="L24" s="17"/>
       <c r="M24" s="14"/>
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
@@ -1677,11 +1677,11 @@
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="18"/>
+      <c r="H25" s="17"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
-      <c r="L25" s="18"/>
+      <c r="L25" s="17"/>
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
@@ -1693,29 +1693,29 @@
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="17"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
-      <c r="L26" s="18"/>
+      <c r="L26" s="17"/>
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="18"/>
+      <c r="H27" s="17"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
-      <c r="L27" s="18"/>
+      <c r="L27" s="17"/>
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
@@ -1726,14 +1726,14 @@
         <v>0</v>
       </c>
       <c r="C28" s="13"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="17"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
-      <c r="L28" s="18"/>
+      <c r="L28" s="17"/>
       <c r="M28" s="14"/>
       <c r="N28" s="14"/>
       <c r="O28" s="14"/>
@@ -1748,14 +1748,14 @@
       <c r="C29" s="7">
         <v>0</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="18"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="17"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
-      <c r="L29" s="18"/>
+      <c r="L29" s="17"/>
       <c r="M29" s="14"/>
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
@@ -1766,14 +1766,14 @@
         <v>0</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="18"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="17"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
-      <c r="L30" s="18"/>
+      <c r="L30" s="17"/>
       <c r="M30" s="14"/>
       <c r="N30" s="14"/>
       <c r="O30" s="14"/>
@@ -1785,21 +1785,21 @@
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="18"/>
+      <c r="H31" s="17"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
-      <c r="L31" s="18"/>
+      <c r="L31" s="17"/>
       <c r="M31" s="14"/>
       <c r="N31" s="14"/>
       <c r="O31" s="14"/>
     </row>
     <row r="33" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
@@ -1818,9 +1818,9 @@
         <v>0</v>
       </c>
       <c r="C34" s="13"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="20"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="19"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -1840,9 +1840,9 @@
       <c r="C35" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="25"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="24"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -1858,9 +1858,9 @@
         <v>0</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="22"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -1874,15 +1874,15 @@
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
-      <c r="D37" s="18"/>
+      <c r="D37" s="17"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="18"/>
+      <c r="H37" s="17"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
-      <c r="L37" s="18"/>
+      <c r="L37" s="17"/>
       <c r="M37" s="14"/>
       <c r="N37" s="14"/>
       <c r="O37" s="14"/>
@@ -1891,34 +1891,34 @@
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="18"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="18"/>
+      <c r="H38" s="17"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="18"/>
+      <c r="L38" s="17"/>
       <c r="M38" s="14"/>
       <c r="N38" s="14"/>
       <c r="O38" s="14"/>
     </row>
     <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="18"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="17"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="18"/>
+      <c r="H39" s="17"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
-      <c r="L39" s="18"/>
+      <c r="L39" s="17"/>
       <c r="M39" s="14"/>
       <c r="N39" s="14"/>
       <c r="O39" s="14"/>
@@ -1929,15 +1929,15 @@
         <v>0</v>
       </c>
       <c r="C40" s="13"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="18"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="17"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
-      <c r="L40" s="18"/>
+      <c r="L40" s="17"/>
       <c r="M40" s="14"/>
       <c r="N40" s="14"/>
       <c r="O40" s="14"/>
@@ -1952,15 +1952,15 @@
       <c r="C41" s="7">
         <v>0</v>
       </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="18"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="17"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
       <c r="K41" s="14"/>
-      <c r="L41" s="18"/>
+      <c r="L41" s="17"/>
       <c r="M41" s="14"/>
       <c r="N41" s="14"/>
       <c r="O41" s="14"/>
@@ -1971,15 +1971,15 @@
         <v>0</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="18"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="17"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
-      <c r="L42" s="18"/>
+      <c r="L42" s="17"/>
       <c r="M42" s="14"/>
       <c r="N42" s="14"/>
       <c r="O42" s="14"/>
@@ -1988,15 +1988,15 @@
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
-      <c r="D43" s="18"/>
+      <c r="D43" s="17"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
-      <c r="H43" s="18"/>
+      <c r="H43" s="17"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
-      <c r="L43" s="18"/>
+      <c r="L43" s="17"/>
       <c r="M43" s="14"/>
       <c r="N43" s="14"/>
       <c r="O43" s="14"/>
@@ -2005,34 +2005,34 @@
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
-      <c r="D44" s="18"/>
+      <c r="D44" s="17"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="18"/>
+      <c r="H44" s="17"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
       <c r="K44" s="14"/>
-      <c r="L44" s="18"/>
+      <c r="L44" s="17"/>
       <c r="M44" s="14"/>
       <c r="N44" s="14"/>
       <c r="O44" s="14"/>
     </row>
     <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="17"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
-      <c r="H45" s="18"/>
+      <c r="H45" s="17"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
       <c r="K45" s="14"/>
-      <c r="L45" s="18"/>
+      <c r="L45" s="17"/>
       <c r="M45" s="14"/>
       <c r="N45" s="14"/>
       <c r="O45" s="14"/>
@@ -2043,15 +2043,15 @@
         <v>0</v>
       </c>
       <c r="C46" s="13"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="18"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="17"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
       <c r="K46" s="14"/>
-      <c r="L46" s="18"/>
+      <c r="L46" s="17"/>
       <c r="M46" s="14"/>
       <c r="N46" s="14"/>
       <c r="O46" s="14"/>
@@ -2066,15 +2066,15 @@
       <c r="C47" s="7">
         <v>0</v>
       </c>
-      <c r="D47" s="18"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="18"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="17"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
       <c r="K47" s="14"/>
-      <c r="L47" s="18"/>
+      <c r="L47" s="17"/>
       <c r="M47" s="14"/>
       <c r="N47" s="14"/>
       <c r="O47" s="14"/>
@@ -2085,15 +2085,15 @@
         <v>0</v>
       </c>
       <c r="C48" s="12"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="18"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="17"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
       <c r="K48" s="14"/>
-      <c r="L48" s="18"/>
+      <c r="L48" s="17"/>
       <c r="M48" s="14"/>
       <c r="N48" s="14"/>
       <c r="O48" s="14"/>
@@ -2102,15 +2102,15 @@
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
-      <c r="D49" s="18"/>
+      <c r="D49" s="17"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
-      <c r="H49" s="18"/>
+      <c r="H49" s="17"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
-      <c r="L49" s="18"/>
+      <c r="L49" s="17"/>
       <c r="M49" s="14"/>
       <c r="N49" s="14"/>
       <c r="O49" s="14"/>
@@ -2119,34 +2119,34 @@
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
-      <c r="D50" s="18"/>
+      <c r="D50" s="17"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
-      <c r="H50" s="18"/>
+      <c r="H50" s="17"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
-      <c r="L50" s="18"/>
+      <c r="L50" s="17"/>
       <c r="M50" s="14"/>
       <c r="N50" s="14"/>
       <c r="O50" s="14"/>
     </row>
     <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="18"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="17"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
       <c r="G51" s="14"/>
-      <c r="H51" s="18"/>
+      <c r="H51" s="17"/>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
       <c r="K51" s="14"/>
-      <c r="L51" s="18"/>
+      <c r="L51" s="17"/>
       <c r="M51" s="14"/>
       <c r="N51" s="14"/>
       <c r="O51" s="14"/>
@@ -2157,15 +2157,15 @@
         <v>0</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="18"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="17"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
       <c r="K52" s="14"/>
-      <c r="L52" s="18"/>
+      <c r="L52" s="17"/>
       <c r="M52" s="14"/>
       <c r="N52" s="14"/>
       <c r="O52" s="14"/>
@@ -2180,15 +2180,15 @@
       <c r="C53" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D53" s="18"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="18"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="17"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
       <c r="K53" s="14"/>
-      <c r="L53" s="18"/>
+      <c r="L53" s="17"/>
       <c r="M53" s="14"/>
       <c r="N53" s="14"/>
       <c r="O53" s="14"/>
@@ -2199,15 +2199,15 @@
         <v>0</v>
       </c>
       <c r="C54" s="12"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="18"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="17"/>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
       <c r="K54" s="14"/>
-      <c r="L54" s="18"/>
+      <c r="L54" s="17"/>
       <c r="M54" s="14"/>
       <c r="N54" s="14"/>
       <c r="O54" s="14"/>
@@ -2216,25 +2216,25 @@
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
-      <c r="D55" s="18"/>
+      <c r="D55" s="17"/>
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
-      <c r="H55" s="18"/>
+      <c r="H55" s="17"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
       <c r="K55" s="14"/>
-      <c r="L55" s="18"/>
+      <c r="L55" s="17"/>
       <c r="M55" s="14"/>
       <c r="N55" s="14"/>
       <c r="O55" s="14"/>
     </row>
     <row r="57" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="41"/>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
@@ -2253,9 +2253,9 @@
         <v>0</v>
       </c>
       <c r="C58" s="13"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="20"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="19"/>
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
@@ -2275,9 +2275,9 @@
       <c r="C59" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E59" s="28"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="25"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="24"/>
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
@@ -2293,9 +2293,9 @@
         <v>0</v>
       </c>
       <c r="C60" s="12"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="22"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="21"/>
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
@@ -2309,15 +2309,15 @@
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="18"/>
+      <c r="D61" s="17"/>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
-      <c r="H61" s="18"/>
+      <c r="H61" s="17"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
       <c r="K61" s="14"/>
-      <c r="L61" s="18"/>
+      <c r="L61" s="17"/>
       <c r="M61" s="14"/>
       <c r="N61" s="14"/>
       <c r="O61" s="14"/>
@@ -2326,34 +2326,34 @@
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
-      <c r="D62" s="18"/>
+      <c r="D62" s="17"/>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
       <c r="G62" s="14"/>
-      <c r="H62" s="18"/>
+      <c r="H62" s="17"/>
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
       <c r="K62" s="14"/>
-      <c r="L62" s="18"/>
+      <c r="L62" s="17"/>
       <c r="M62" s="14"/>
       <c r="N62" s="14"/>
       <c r="O62" s="14"/>
     </row>
     <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="18"/>
+      <c r="B63" s="41"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="17"/>
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
-      <c r="H63" s="18"/>
+      <c r="H63" s="17"/>
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
       <c r="K63" s="14"/>
-      <c r="L63" s="18"/>
+      <c r="L63" s="17"/>
       <c r="M63" s="14"/>
       <c r="N63" s="14"/>
       <c r="O63" s="14"/>
@@ -2364,15 +2364,15 @@
         <v>0</v>
       </c>
       <c r="C64" s="13"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="18"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="17"/>
       <c r="I64" s="14"/>
       <c r="J64" s="14"/>
       <c r="K64" s="14"/>
-      <c r="L64" s="18"/>
+      <c r="L64" s="17"/>
       <c r="M64" s="14"/>
       <c r="N64" s="14"/>
       <c r="O64" s="14"/>
@@ -2387,15 +2387,15 @@
       <c r="C65" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="18"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="17"/>
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
       <c r="K65" s="14"/>
-      <c r="L65" s="18"/>
+      <c r="L65" s="17"/>
       <c r="M65" s="14"/>
       <c r="N65" s="14"/>
       <c r="O65" s="14"/>
@@ -2406,15 +2406,15 @@
         <v>0</v>
       </c>
       <c r="C66" s="12"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="22"/>
-      <c r="H66" s="18"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="17"/>
       <c r="I66" s="14"/>
       <c r="J66" s="14"/>
       <c r="K66" s="14"/>
-      <c r="L66" s="18"/>
+      <c r="L66" s="17"/>
       <c r="M66" s="14"/>
       <c r="N66" s="14"/>
       <c r="O66" s="14"/>
@@ -2423,15 +2423,15 @@
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
-      <c r="D67" s="18"/>
+      <c r="D67" s="17"/>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
-      <c r="H67" s="18"/>
+      <c r="H67" s="17"/>
       <c r="I67" s="14"/>
       <c r="J67" s="14"/>
       <c r="K67" s="14"/>
-      <c r="L67" s="18"/>
+      <c r="L67" s="17"/>
       <c r="M67" s="14"/>
       <c r="N67" s="14"/>
       <c r="O67" s="14"/>
@@ -2440,34 +2440,34 @@
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
-      <c r="D68" s="18"/>
+      <c r="D68" s="17"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
-      <c r="H68" s="18"/>
+      <c r="H68" s="17"/>
       <c r="I68" s="14"/>
       <c r="J68" s="14"/>
       <c r="K68" s="14"/>
-      <c r="L68" s="18"/>
+      <c r="L68" s="17"/>
       <c r="M68" s="14"/>
       <c r="N68" s="14"/>
       <c r="O68" s="14"/>
     </row>
     <row r="69" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="18"/>
+      <c r="B69" s="41"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="17"/>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
       <c r="G69" s="14"/>
-      <c r="H69" s="18"/>
+      <c r="H69" s="17"/>
       <c r="I69" s="14"/>
       <c r="J69" s="14"/>
       <c r="K69" s="14"/>
-      <c r="L69" s="18"/>
+      <c r="L69" s="17"/>
       <c r="M69" s="14"/>
       <c r="N69" s="14"/>
       <c r="O69" s="14"/>
@@ -2478,15 +2478,15 @@
         <v>0</v>
       </c>
       <c r="C70" s="13"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="18"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="17"/>
       <c r="I70" s="14"/>
       <c r="J70" s="14"/>
       <c r="K70" s="14"/>
-      <c r="L70" s="18"/>
+      <c r="L70" s="17"/>
       <c r="M70" s="14"/>
       <c r="N70" s="14"/>
       <c r="O70" s="14"/>
@@ -2501,15 +2501,15 @@
       <c r="C71" s="7">
         <v>0</v>
       </c>
-      <c r="D71" s="18"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="40"/>
-      <c r="H71" s="18"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="36"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="17"/>
       <c r="I71" s="14"/>
       <c r="J71" s="14"/>
       <c r="K71" s="14"/>
-      <c r="L71" s="18"/>
+      <c r="L71" s="17"/>
       <c r="M71" s="14"/>
       <c r="N71" s="14"/>
       <c r="O71" s="14"/>
@@ -2520,15 +2520,15 @@
         <v>0</v>
       </c>
       <c r="C72" s="12"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="26"/>
-      <c r="G72" s="22"/>
-      <c r="H72" s="18"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="17"/>
       <c r="I72" s="14"/>
       <c r="J72" s="14"/>
       <c r="K72" s="14"/>
-      <c r="L72" s="18"/>
+      <c r="L72" s="17"/>
       <c r="M72" s="14"/>
       <c r="N72" s="14"/>
       <c r="O72" s="14"/>
@@ -2537,15 +2537,15 @@
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
-      <c r="D73" s="18"/>
+      <c r="D73" s="17"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
       <c r="G73" s="14"/>
-      <c r="H73" s="18"/>
+      <c r="H73" s="17"/>
       <c r="I73" s="14"/>
       <c r="J73" s="14"/>
       <c r="K73" s="14"/>
-      <c r="L73" s="18"/>
+      <c r="L73" s="17"/>
       <c r="M73" s="14"/>
       <c r="N73" s="14"/>
       <c r="O73" s="14"/>
@@ -2554,34 +2554,34 @@
       <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
-      <c r="D74" s="18"/>
+      <c r="D74" s="17"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
       <c r="G74" s="14"/>
-      <c r="H74" s="18"/>
+      <c r="H74" s="17"/>
       <c r="I74" s="14"/>
       <c r="J74" s="14"/>
       <c r="K74" s="14"/>
-      <c r="L74" s="18"/>
+      <c r="L74" s="17"/>
       <c r="M74" s="14"/>
       <c r="N74" s="14"/>
       <c r="O74" s="14"/>
     </row>
     <row r="75" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="18"/>
+      <c r="B75" s="41"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="17"/>
       <c r="E75" s="14"/>
       <c r="F75" s="14"/>
       <c r="G75" s="14"/>
-      <c r="H75" s="18"/>
+      <c r="H75" s="17"/>
       <c r="I75" s="14"/>
       <c r="J75" s="14"/>
       <c r="K75" s="14"/>
-      <c r="L75" s="18"/>
+      <c r="L75" s="17"/>
       <c r="M75" s="14"/>
       <c r="N75" s="14"/>
       <c r="O75" s="14"/>
@@ -2592,15 +2592,15 @@
         <v>0</v>
       </c>
       <c r="C76" s="13"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="20"/>
-      <c r="H76" s="18"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="17"/>
       <c r="I76" s="14"/>
       <c r="J76" s="14"/>
       <c r="K76" s="14"/>
-      <c r="L76" s="18"/>
+      <c r="L76" s="17"/>
       <c r="M76" s="14"/>
       <c r="N76" s="14"/>
       <c r="O76" s="14"/>
@@ -2615,15 +2615,15 @@
       <c r="C77" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D77" s="18"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="38"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="18"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="17"/>
       <c r="I77" s="14"/>
       <c r="J77" s="14"/>
       <c r="K77" s="14"/>
-      <c r="L77" s="18"/>
+      <c r="L77" s="17"/>
       <c r="M77" s="14"/>
       <c r="N77" s="14"/>
       <c r="O77" s="14"/>
@@ -2634,15 +2634,15 @@
         <v>0</v>
       </c>
       <c r="C78" s="12"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="39"/>
-      <c r="G78" s="22"/>
-      <c r="H78" s="18"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="17"/>
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
       <c r="K78" s="14"/>
-      <c r="L78" s="18"/>
+      <c r="L78" s="17"/>
       <c r="M78" s="14"/>
       <c r="N78" s="14"/>
       <c r="O78" s="14"/>
@@ -2651,25 +2651,25 @@
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
-      <c r="D79" s="18"/>
+      <c r="D79" s="17"/>
       <c r="E79" s="14"/>
       <c r="F79" s="14"/>
       <c r="G79" s="14"/>
-      <c r="H79" s="18"/>
+      <c r="H79" s="17"/>
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
       <c r="K79" s="14"/>
-      <c r="L79" s="18"/>
+      <c r="L79" s="17"/>
       <c r="M79" s="14"/>
       <c r="N79" s="14"/>
       <c r="O79" s="14"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="16" t="s">
+      <c r="A81" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
+      <c r="B81" s="41"/>
+      <c r="C81" s="41"/>
       <c r="E81" s="15"/>
       <c r="F81" s="15"/>
       <c r="G81" s="15"/>
@@ -2680,9 +2680,9 @@
         <v>0</v>
       </c>
       <c r="C82" s="13"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="20"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="19"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
@@ -2694,9 +2694,9 @@
       <c r="C83" s="7">
         <v>0</v>
       </c>
-      <c r="E83" s="28"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="40"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="36"/>
+      <c r="G83" s="38"/>
     </row>
     <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="11"/>
@@ -2704,16 +2704,16 @@
         <v>0</v>
       </c>
       <c r="C84" s="12"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="26"/>
-      <c r="G84" s="22"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="25"/>
+      <c r="G84" s="21"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="16" t="s">
+      <c r="A87" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="B87" s="16"/>
-      <c r="C87" s="16"/>
+      <c r="B87" s="41"/>
+      <c r="C87" s="41"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="10"/>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="C88" s="13"/>
       <c r="E88" s="2"/>
-      <c r="F88" s="35"/>
+      <c r="F88" s="34"/>
       <c r="G88" s="4"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -2736,7 +2736,7 @@
         <v>0</v>
       </c>
       <c r="E89" s="5"/>
-      <c r="F89" s="38"/>
+      <c r="F89" s="36"/>
       <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2746,11 +2746,12 @@
       </c>
       <c r="C90" s="12"/>
       <c r="E90" s="8"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="33"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A51:C51"/>
     <mergeCell ref="A87:C87"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
@@ -2767,7 +2768,6 @@
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A51:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2777,335 +2777,335 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE3672E-34EA-4881-9041-23FAFDDA37D1}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="10.90625" style="41"/>
+    <col min="1" max="16384" width="10.90625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="E1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="E3" s="37" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="E3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="25"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="24"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="29"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="22"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="21"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="E9" s="37" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="E9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="25"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="24"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="21"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="22"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="21"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="E15" s="37" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="E15" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="33"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
+      <c r="C18" s="32"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="E21" s="37" t="s">
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="E21" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
-      <c r="B22" s="35"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="4"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="40"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="38"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="8"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="33"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="32"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="E27" s="37" t="s">
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="E27" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="19"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="20"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="19"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="40"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="38"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="21"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="22"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="21"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="E33" s="37" t="s">
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="E33" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="19"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="20"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="19"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="24"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="40"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="38"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="21"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="22"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="21"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="E39" s="37" t="s">
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="E39" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="19"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="20"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="19"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="24"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="25"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="24"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="21"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="22"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="21"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="E45" s="37" t="s">
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="E45" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
-      <c r="B46" s="35"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="4"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
-      <c r="B47" s="38"/>
+      <c r="B47" s="36"/>
       <c r="C47" s="7"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="8"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="33"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="32"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E3:G6"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:G12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:G18"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="E21:G24"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E27:G30"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="E33:G36"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="E39:G42"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="E45:G48"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="E15:G18"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="E21:G24"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E27:G30"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E3:G6"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Affichage de la carte du labyrinthe lorsque le joueur ne fait rien pendant 1 seconde : OK
</commit_message>
<xml_diff>
--- a/Types de Murs Possibles.xlsx
+++ b/Types de Murs Possibles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\INFO5\Bibliotheque_de_developpement_multimedia\Labyrinthe3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1830FBD-E9F8-4497-9C32-29A8EFC56B6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF5D87-2290-4FEF-9B0F-0B50006D42F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="3" xr2:uid="{3C8390C5-9047-4A19-85FD-4E1F16ACA795}"/>
   </bookViews>
@@ -2751,6 +2751,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A45:C45"/>
     <mergeCell ref="A51:C51"/>
     <mergeCell ref="A87:C87"/>
     <mergeCell ref="A1:C1"/>
@@ -2766,8 +2768,6 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A45:C45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2777,8 +2777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE3672E-34EA-4881-9041-23FAFDDA37D1}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>